<commit_message>
adding results for every exchange rate
</commit_message>
<xml_diff>
--- a/1Article/ResultsWithHurstExponent.xlsx
+++ b/1Article/ResultsWithHurstExponent.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robszo\Desktop\PierwszyArtykuł\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robszo\Desktop\phdproject\TimeSeriesForecasting\articles\article1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1331" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1331" uniqueCount="66">
   <si>
     <t>AUDCADask</t>
   </si>
@@ -205,6 +205,36 @@
   <si>
     <t>EURUSDask</t>
   </si>
+  <si>
+    <t xml:space="preserve">0.1 to 0.2 </t>
+  </si>
+  <si>
+    <t>0.0 to 0.1</t>
+  </si>
+  <si>
+    <t>0.2 to 0.3</t>
+  </si>
+  <si>
+    <t>0.3 to 0.4</t>
+  </si>
+  <si>
+    <t>0.4 to 0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5 to 0.6  </t>
+  </si>
+  <si>
+    <t>0.7 to 0.8</t>
+  </si>
+  <si>
+    <t>0.6 to 0.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8 to 0.9 </t>
+  </si>
+  <si>
+    <t>0.9 to 1.0</t>
+  </si>
 </sst>
 </file>
 
@@ -230,7 +260,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -258,6 +288,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -459,7 +495,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
@@ -494,6 +530,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -527,137 +564,17 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:buClrTx/>
-              <a:buSzTx/>
-              <a:buFontTx/>
-              <a:buNone/>
-              <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pl-PL" sz="1800" b="1" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Mean forecast amape error for different Hurst ratio segements for currency pairs</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US">
-              <a:effectLst/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:buClrTx/>
-              <a:buSzTx/>
-              <a:buFontTx/>
-              <a:buNone/>
-              <a:tabLst/>
-              <a:defRPr>
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:sysClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="6.2127910463010881E-2"/>
+          <c:x val="0.12242551275603003"/>
           <c:y val="5.3137994847418268E-2"/>
-          <c:w val="0.92919717198719654"/>
-          <c:h val="0.86813285436094689"/>
+          <c:w val="0.70346710419420955"/>
+          <c:h val="0.79747233208752133"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -680,7 +597,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="FFFF00"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -695,25 +612,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>From 0.0 to 0.1</c:v>
+                  <c:v>0.0 to 0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>From 0.1 to 0.2 </c:v>
+                  <c:v>0.1 to 0.2 </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>From 0.2 to 0.3</c:v>
+                  <c:v>0.2 to 0.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>From 0.3 to 0.4</c:v>
+                  <c:v>0.3 to 0.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>From 0.4 to 0.5</c:v>
+                  <c:v>0.4 to 0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>From 0.5 to 0.6  </c:v>
+                  <c:v>0.5 to 0.6  </c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>From 0.6 to 0.7</c:v>
+                  <c:v>0.6 to 0.7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -767,7 +684,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="FFC000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -782,25 +699,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>From 0.0 to 0.1</c:v>
+                  <c:v>0.0 to 0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>From 0.1 to 0.2 </c:v>
+                  <c:v>0.1 to 0.2 </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>From 0.2 to 0.3</c:v>
+                  <c:v>0.2 to 0.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>From 0.3 to 0.4</c:v>
+                  <c:v>0.3 to 0.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>From 0.4 to 0.5</c:v>
+                  <c:v>0.4 to 0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>From 0.5 to 0.6  </c:v>
+                  <c:v>0.5 to 0.6  </c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>From 0.6 to 0.7</c:v>
+                  <c:v>0.6 to 0.7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -854,7 +771,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -869,25 +786,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>From 0.0 to 0.1</c:v>
+                  <c:v>0.0 to 0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>From 0.1 to 0.2 </c:v>
+                  <c:v>0.1 to 0.2 </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>From 0.2 to 0.3</c:v>
+                  <c:v>0.2 to 0.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>From 0.3 to 0.4</c:v>
+                  <c:v>0.3 to 0.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>From 0.4 to 0.5</c:v>
+                  <c:v>0.4 to 0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>From 0.5 to 0.6  </c:v>
+                  <c:v>0.5 to 0.6  </c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>From 0.6 to 0.7</c:v>
+                  <c:v>0.6 to 0.7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -941,7 +858,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -956,25 +873,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>From 0.0 to 0.1</c:v>
+                  <c:v>0.0 to 0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>From 0.1 to 0.2 </c:v>
+                  <c:v>0.1 to 0.2 </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>From 0.2 to 0.3</c:v>
+                  <c:v>0.2 to 0.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>From 0.3 to 0.4</c:v>
+                  <c:v>0.3 to 0.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>From 0.4 to 0.5</c:v>
+                  <c:v>0.4 to 0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>From 0.5 to 0.6  </c:v>
+                  <c:v>0.5 to 0.6  </c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>From 0.6 to 0.7</c:v>
+                  <c:v>0.6 to 0.7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1028,7 +945,9 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent5"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1043,25 +962,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>From 0.0 to 0.1</c:v>
+                  <c:v>0.0 to 0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>From 0.1 to 0.2 </c:v>
+                  <c:v>0.1 to 0.2 </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>From 0.2 to 0.3</c:v>
+                  <c:v>0.2 to 0.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>From 0.3 to 0.4</c:v>
+                  <c:v>0.3 to 0.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>From 0.4 to 0.5</c:v>
+                  <c:v>0.4 to 0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>From 0.5 to 0.6  </c:v>
+                  <c:v>0.5 to 0.6  </c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>From 0.6 to 0.7</c:v>
+                  <c:v>0.6 to 0.7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1115,7 +1034,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:srgbClr val="00B0F0"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1130,25 +1049,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>From 0.0 to 0.1</c:v>
+                  <c:v>0.0 to 0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>From 0.1 to 0.2 </c:v>
+                  <c:v>0.1 to 0.2 </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>From 0.2 to 0.3</c:v>
+                  <c:v>0.2 to 0.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>From 0.3 to 0.4</c:v>
+                  <c:v>0.3 to 0.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>From 0.4 to 0.5</c:v>
+                  <c:v>0.4 to 0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>From 0.5 to 0.6  </c:v>
+                  <c:v>0.5 to 0.6  </c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>From 0.6 to 0.7</c:v>
+                  <c:v>0.6 to 0.7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1202,9 +1121,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
+                <a:srgbClr val="7030A0"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1219,25 +1136,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>From 0.0 to 0.1</c:v>
+                  <c:v>0.0 to 0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>From 0.1 to 0.2 </c:v>
+                  <c:v>0.1 to 0.2 </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>From 0.2 to 0.3</c:v>
+                  <c:v>0.2 to 0.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>From 0.3 to 0.4</c:v>
+                  <c:v>0.3 to 0.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>From 0.4 to 0.5</c:v>
+                  <c:v>0.4 to 0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>From 0.5 to 0.6  </c:v>
+                  <c:v>0.5 to 0.6  </c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>From 0.6 to 0.7</c:v>
+                  <c:v>0.6 to 0.7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1283,84 +1200,16 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-71675904"/>
-        <c:axId val="-71669376"/>
+        <c:axId val="2076054864"/>
+        <c:axId val="2076052144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-71675904"/>
+        <c:axId val="2076054864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="pl-PL" sz="2400"/>
-                  <a:t>Hurst</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="pl-PL" sz="2400" baseline="0"/>
-                  <a:t> ratio segments</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" sz="2400"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0.41622851634959107"/>
-              <c:y val="0.94713196951464096"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1383,7 +1232,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1398,7 +1247,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-71669376"/>
+        <c:crossAx val="2076052144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1406,9 +1255,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-71669376"/>
+        <c:axId val="2076052144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1.2000000000000005E-5"/>
+          <c:min val="2.0000000000000008E-6"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1446,18 +1297,25 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL" sz="1800"/>
-                  <a:t>Mean</a:t>
+                  <a:rPr lang="pl-PL" sz="2800"/>
+                  <a:t>Mean </a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="pl-PL" sz="1800" baseline="0"/>
-                  <a:t> amape error </a:t>
+                  <a:rPr lang="pl-PL" sz="2800" baseline="0"/>
+                  <a:t>AMAPE error</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US" sz="1800"/>
+                <a:endParaRPr lang="en-US" sz="2800"/>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="5.9703424208899679E-3"/>
+              <c:y val="0.3016667271429781"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1487,7 +1345,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.0000000000" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000000" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1503,7 +1361,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1518,7 +1376,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-71675904"/>
+        <c:crossAx val="2076054864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1536,10 +1394,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.75868537577890593"/>
-          <c:y val="6.237452653747623E-2"/>
-          <c:w val="0.18059026941736381"/>
-          <c:h val="0.29401329624216133"/>
+          <c:x val="0.8384701731149693"/>
+          <c:y val="6.3910640202232791E-2"/>
+          <c:w val="0.16103696597365894"/>
+          <c:h val="0.87312239195906971"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1555,7 +1413,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1605,6 +1463,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -1622,78 +1481,17 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="pl-PL" sz="1800" b="1"/>
-              <a:t>Mean forecast</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pl-PL" sz="1800" b="1" baseline="0"/>
-              <a:t> accuracy for different Hurst ratio segements for currency pairs</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1800" b="1"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.1682931464805686E-2"/>
-          <c:y val="5.8398407590293577E-2"/>
-          <c:w val="0.95193366538338886"/>
-          <c:h val="0.85323030214262152"/>
+          <c:x val="9.4700712563240363E-2"/>
+          <c:y val="5.8398362207238756E-2"/>
+          <c:w val="0.72577695801805675"/>
+          <c:h val="0.82154747361643166"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1716,7 +1514,9 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1731,25 +1531,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>From 0.0 to 0.1</c:v>
+                  <c:v>0.0 to 0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>From 0.1 to 0.2 </c:v>
+                  <c:v>0.1 to 0.2 </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>From 0.2 to 0.3</c:v>
+                  <c:v>0.2 to 0.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>From 0.3 to 0.4</c:v>
+                  <c:v>0.3 to 0.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>From 0.4 to 0.5</c:v>
+                  <c:v>0.4 to 0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>From 0.5 to 0.6  </c:v>
+                  <c:v>0.5 to 0.6  </c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>From 0.6 to 0.7</c:v>
+                  <c:v>0.6 to 0.7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1803,7 +1603,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1818,25 +1618,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>From 0.0 to 0.1</c:v>
+                  <c:v>0.0 to 0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>From 0.1 to 0.2 </c:v>
+                  <c:v>0.1 to 0.2 </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>From 0.2 to 0.3</c:v>
+                  <c:v>0.2 to 0.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>From 0.3 to 0.4</c:v>
+                  <c:v>0.3 to 0.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>From 0.4 to 0.5</c:v>
+                  <c:v>0.4 to 0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>From 0.5 to 0.6  </c:v>
+                  <c:v>0.5 to 0.6  </c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>From 0.6 to 0.7</c:v>
+                  <c:v>0.6 to 0.7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1890,7 +1690,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:srgbClr val="FFFF00"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1905,25 +1705,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>From 0.0 to 0.1</c:v>
+                  <c:v>0.0 to 0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>From 0.1 to 0.2 </c:v>
+                  <c:v>0.1 to 0.2 </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>From 0.2 to 0.3</c:v>
+                  <c:v>0.2 to 0.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>From 0.3 to 0.4</c:v>
+                  <c:v>0.3 to 0.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>From 0.4 to 0.5</c:v>
+                  <c:v>0.4 to 0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>From 0.5 to 0.6  </c:v>
+                  <c:v>0.5 to 0.6  </c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>From 0.6 to 0.7</c:v>
+                  <c:v>0.6 to 0.7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1977,7 +1777,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:srgbClr val="FFC000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1992,25 +1792,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>From 0.0 to 0.1</c:v>
+                  <c:v>0.0 to 0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>From 0.1 to 0.2 </c:v>
+                  <c:v>0.1 to 0.2 </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>From 0.2 to 0.3</c:v>
+                  <c:v>0.2 to 0.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>From 0.3 to 0.4</c:v>
+                  <c:v>0.3 to 0.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>From 0.4 to 0.5</c:v>
+                  <c:v>0.4 to 0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>From 0.5 to 0.6  </c:v>
+                  <c:v>0.5 to 0.6  </c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>From 0.6 to 0.7</c:v>
+                  <c:v>0.6 to 0.7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2064,7 +1864,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent5"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2079,25 +1879,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>From 0.0 to 0.1</c:v>
+                  <c:v>0.0 to 0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>From 0.1 to 0.2 </c:v>
+                  <c:v>0.1 to 0.2 </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>From 0.2 to 0.3</c:v>
+                  <c:v>0.2 to 0.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>From 0.3 to 0.4</c:v>
+                  <c:v>0.3 to 0.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>From 0.4 to 0.5</c:v>
+                  <c:v>0.4 to 0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>From 0.5 to 0.6  </c:v>
+                  <c:v>0.5 to 0.6  </c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>From 0.6 to 0.7</c:v>
+                  <c:v>0.6 to 0.7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2151,7 +1951,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:srgbClr val="C00000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2166,25 +1966,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>From 0.0 to 0.1</c:v>
+                  <c:v>0.0 to 0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>From 0.1 to 0.2 </c:v>
+                  <c:v>0.1 to 0.2 </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>From 0.2 to 0.3</c:v>
+                  <c:v>0.2 to 0.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>From 0.3 to 0.4</c:v>
+                  <c:v>0.3 to 0.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>From 0.4 to 0.5</c:v>
+                  <c:v>0.4 to 0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>From 0.5 to 0.6  </c:v>
+                  <c:v>0.5 to 0.6  </c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>From 0.6 to 0.7</c:v>
+                  <c:v>0.6 to 0.7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2238,8 +2038,95 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Zestawienie!$B$2:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.0 to 0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1 to 0.2 </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2 to 0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3 to 0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4 to 0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5 to 0.6  </c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6 to 0.7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Zestawienie!$I$2:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.41312142857142847</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.40469285714285713</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.40005000000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.39622142857142856</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.39058571428571437</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.38357857142857149</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.35298000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Zestawienie!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Linear regression</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -2255,114 +2142,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>From 0.0 to 0.1</c:v>
+                  <c:v>0.0 to 0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>From 0.1 to 0.2 </c:v>
+                  <c:v>0.1 to 0.2 </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>From 0.2 to 0.3</c:v>
+                  <c:v>0.2 to 0.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>From 0.3 to 0.4</c:v>
+                  <c:v>0.3 to 0.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>From 0.4 to 0.5</c:v>
+                  <c:v>0.4 to 0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>From 0.5 to 0.6  </c:v>
+                  <c:v>0.5 to 0.6  </c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>From 0.6 to 0.7</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Zestawienie!$I$2:$I$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.41312142857142847</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.40469285714285713</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.40005000000000007</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.39622142857142856</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.39058571428571437</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.38357857142857149</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.35298000000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Zestawienie!$J$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Linear regression</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Zestawienie!$B$2:$B$8</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>From 0.0 to 0.1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>From 0.1 to 0.2 </c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>From 0.2 to 0.3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>From 0.3 to 0.4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>From 0.4 to 0.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>From 0.5 to 0.6  </c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>From 0.6 to 0.7</c:v>
+                  <c:v>0.6 to 0.7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2416,9 +2214,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
+                <a:srgbClr val="00B0F0"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2433,25 +2229,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>From 0.0 to 0.1</c:v>
+                  <c:v>0.0 to 0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>From 0.1 to 0.2 </c:v>
+                  <c:v>0.1 to 0.2 </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>From 0.2 to 0.3</c:v>
+                  <c:v>0.2 to 0.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>From 0.3 to 0.4</c:v>
+                  <c:v>0.3 to 0.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>From 0.4 to 0.5</c:v>
+                  <c:v>0.4 to 0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>From 0.5 to 0.6  </c:v>
+                  <c:v>0.5 to 0.6  </c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>From 0.6 to 0.7</c:v>
+                  <c:v>0.6 to 0.7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2505,9 +2301,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
+                <a:srgbClr val="7030A0"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2522,25 +2316,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>From 0.0 to 0.1</c:v>
+                  <c:v>0.0 to 0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>From 0.1 to 0.2 </c:v>
+                  <c:v>0.1 to 0.2 </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>From 0.2 to 0.3</c:v>
+                  <c:v>0.2 to 0.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>From 0.3 to 0.4</c:v>
+                  <c:v>0.3 to 0.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>From 0.4 to 0.5</c:v>
+                  <c:v>0.4 to 0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>From 0.5 to 0.6  </c:v>
+                  <c:v>0.5 to 0.6  </c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>From 0.6 to 0.7</c:v>
+                  <c:v>0.6 to 0.7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2586,11 +2380,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-71668832"/>
-        <c:axId val="-71671008"/>
+        <c:axId val="2076055952"/>
+        <c:axId val="2076053232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-71668832"/>
+        <c:axId val="2076055952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2617,7 +2411,7 @@
                   <a:buFontTx/>
                   <a:buNone/>
                   <a:tabLst/>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000">
                         <a:lumMod val="65000"/>
@@ -2629,75 +2423,26 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="pl-PL" sz="1000" b="0" i="0" baseline="0">
-                  <a:effectLst/>
-                </a:endParaRPr>
-              </a:p>
-              <a:p>
-                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-                  <a:lnSpc>
-                    <a:spcPct val="100000"/>
-                  </a:lnSpc>
-                  <a:spcBef>
-                    <a:spcPts val="0"/>
-                  </a:spcBef>
-                  <a:spcAft>
-                    <a:spcPts val="0"/>
-                  </a:spcAft>
-                  <a:buClrTx/>
-                  <a:buSzTx/>
-                  <a:buFontTx/>
-                  <a:buNone/>
-                  <a:tabLst/>
-                  <a:defRPr>
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:sysClr>
-                    </a:solidFill>
-                  </a:defRPr>
-                </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL" sz="1800" b="0" i="0" baseline="0">
-                    <a:effectLst/>
-                  </a:rPr>
-                  <a:t>Hurst ratio segments</a:t>
+                  <a:rPr lang="pl-PL" sz="2400"/>
+                  <a:t>Segments</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US">
-                  <a:effectLst/>
-                </a:endParaRPr>
-              </a:p>
-              <a:p>
-                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-                  <a:lnSpc>
-                    <a:spcPct val="100000"/>
-                  </a:lnSpc>
-                  <a:spcBef>
-                    <a:spcPts val="0"/>
-                  </a:spcBef>
-                  <a:spcAft>
-                    <a:spcPts val="0"/>
-                  </a:spcAft>
-                  <a:buClrTx/>
-                  <a:buSzTx/>
-                  <a:buFontTx/>
-                  <a:buNone/>
-                  <a:tabLst/>
-                  <a:defRPr>
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:sysClr>
-                    </a:solidFill>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="2400" baseline="0"/>
+                  <a:t> of the Hurst exponent</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="2400"/>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.31135740973819948"/>
+              <c:y val="0.9536472978835373"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2725,7 +2470,7 @@
                 <a:buFontTx/>
                 <a:buNone/>
                 <a:tabLst/>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000">
                       <a:lumMod val="65000"/>
@@ -2763,7 +2508,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2778,7 +2523,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-71671008"/>
+        <c:crossAx val="2076053232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2786,9 +2531,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-71671008"/>
+        <c:axId val="2076053232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0.70000000000000007"/>
+          <c:min val="0.1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2813,7 +2560,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -2826,12 +2573,12 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL" sz="1800" b="0" i="0" baseline="0">
+                  <a:rPr lang="pl-PL" sz="2400" b="0" i="0" baseline="0">
                     <a:effectLst/>
                   </a:rPr>
-                  <a:t>Mean forecasting accuracy level </a:t>
+                  <a:t>Mean forecasting accuracy </a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US">
+                <a:endParaRPr lang="en-US" sz="2400">
                   <a:effectLst/>
                 </a:endParaRPr>
               </a:p>
@@ -2858,7 +2605,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -2890,7 +2637,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2905,7 +2652,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-71668832"/>
+        <c:crossAx val="2076055952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2919,7 +2666,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.8213544534955346"/>
+          <c:y val="1.1631012391637472E-2"/>
+          <c:w val="0.17756271139854005"/>
+          <c:h val="0.92755797452345723"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2933,7 +2689,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -4519,11 +4275,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-150152128"/>
-        <c:axId val="-10166640"/>
+        <c:axId val="2076056496"/>
+        <c:axId val="2076057040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-150152128"/>
+        <c:axId val="2076056496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4627,7 +4383,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-10166640"/>
+        <c:crossAx val="2076057040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4635,7 +4391,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-10166640"/>
+        <c:axId val="2076057040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4747,7 +4503,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-150152128"/>
+        <c:crossAx val="2076056496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6509,16 +6265,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>28576</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>693964</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>1362</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>114</xdr:row>
-      <xdr:rowOff>104776</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>138793</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>77562</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6541,16 +6297,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>228599</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>628648</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:rowOff>129948</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>247649</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>13607</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>126052</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6573,6 +6329,44 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.30411</cdr:x>
+      <cdr:y>0.92479</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.61971</cdr:x>
+      <cdr:y>1</cdr:y>
+    </cdr:to>
+    <cdr:pic>
+      <cdr:nvPicPr>
+        <cdr:cNvPr id="3" name="chart"/>
+        <cdr:cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cdr:cNvPicPr>
+      </cdr:nvPicPr>
+      <cdr:blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </cdr:blipFill>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4544403" y="7645854"/>
+          <a:ext cx="4716220" cy="621846"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+    </cdr:pic>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -6870,10 +6664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:Q114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="C48" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W68" sqref="W68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6928,7 +6722,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="C2">
         <f>LogisticRegression!B2</f>
@@ -6973,7 +6767,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="C3">
         <f>LogisticRegression!B3</f>
@@ -7018,7 +6812,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="C4">
         <f>LogisticRegression!B4</f>
@@ -7063,7 +6857,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="C5">
         <f>LogisticRegression!B5</f>
@@ -7108,7 +6902,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="C6">
         <f>LogisticRegression!B6</f>
@@ -7153,7 +6947,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="C7">
         <f>LogisticRegression!B7</f>
@@ -7198,7 +6992,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="C8">
         <f>LogisticRegression!B8</f>
@@ -7243,7 +7037,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="C9" t="e">
         <f>LogisticRegression!B9</f>
@@ -7288,7 +7082,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="C10" t="e">
         <f>LogisticRegression!B10</f>
@@ -7333,7 +7127,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="C11" t="e">
         <f>LogisticRegression!B11</f>
@@ -7401,7 +7195,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="C15" s="24">
         <f>ARMA!B14</f>
@@ -7434,7 +7228,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="C16" s="24">
         <f>ARMA!B15</f>
@@ -7465,9 +7259,9 @@
         <v>9.0700000000000013E-6</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="C17" s="24">
         <f>ARMA!B16</f>
@@ -7498,9 +7292,9 @@
         <v>7.0785714285714292E-6</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="C18" s="24">
         <f>ARMA!B17</f>
@@ -7531,9 +7325,9 @@
         <v>6.5971428571428562E-6</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="C19" s="24">
         <f>ARMA!B18</f>
@@ -7564,9 +7358,9 @@
         <v>6.0092857142857151E-6</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="C20" s="24">
         <f>ARMA!B19</f>
@@ -7597,9 +7391,9 @@
         <v>5.1621428571428572E-6</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="C21" s="24">
         <f>ARMA!B20</f>
@@ -7630,9 +7424,9 @@
         <v>3.5959999999999995E-6</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="C22" t="e">
         <f>ARMA!B21</f>
@@ -7663,9 +7457,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="C23" t="e">
         <f>ARMA!B22</f>
@@ -7696,9 +7490,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="C24" t="e">
         <f>ARMA!B23</f>
@@ -7724,6 +7518,1519 @@
         <f>ExpSmooth!B23</f>
         <v>#DIV/0!</v>
       </c>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="26"/>
+      <c r="O26" s="26"/>
+      <c r="P26" s="26"/>
+      <c r="Q26" s="26"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="26"/>
+      <c r="M27" s="26"/>
+      <c r="N27" s="26"/>
+      <c r="O27" s="26"/>
+      <c r="P27" s="26"/>
+      <c r="Q27" s="26"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="26"/>
+      <c r="M28" s="26"/>
+      <c r="N28" s="26"/>
+      <c r="O28" s="26"/>
+      <c r="P28" s="26"/>
+      <c r="Q28" s="26"/>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="26"/>
+      <c r="L29" s="26"/>
+      <c r="M29" s="26"/>
+      <c r="N29" s="26"/>
+      <c r="O29" s="26"/>
+      <c r="P29" s="26"/>
+      <c r="Q29" s="26"/>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="26"/>
+      <c r="M30" s="26"/>
+      <c r="N30" s="26"/>
+      <c r="O30" s="26"/>
+      <c r="P30" s="26"/>
+      <c r="Q30" s="26"/>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="26"/>
+      <c r="M31" s="26"/>
+      <c r="N31" s="26"/>
+      <c r="O31" s="26"/>
+      <c r="P31" s="26"/>
+      <c r="Q31" s="26"/>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="26"/>
+      <c r="N32" s="26"/>
+      <c r="O32" s="26"/>
+      <c r="P32" s="26"/>
+      <c r="Q32" s="26"/>
+    </row>
+    <row r="33" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="26"/>
+      <c r="K33" s="26"/>
+      <c r="L33" s="26"/>
+      <c r="M33" s="26"/>
+      <c r="N33" s="26"/>
+      <c r="O33" s="26"/>
+      <c r="P33" s="26"/>
+      <c r="Q33" s="26"/>
+    </row>
+    <row r="34" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="26"/>
+      <c r="K34" s="26"/>
+      <c r="L34" s="26"/>
+      <c r="M34" s="26"/>
+      <c r="N34" s="26"/>
+      <c r="O34" s="26"/>
+      <c r="P34" s="26"/>
+      <c r="Q34" s="26"/>
+    </row>
+    <row r="35" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="26"/>
+      <c r="K35" s="26"/>
+      <c r="L35" s="26"/>
+      <c r="M35" s="26"/>
+      <c r="N35" s="26"/>
+      <c r="O35" s="26"/>
+      <c r="P35" s="26"/>
+      <c r="Q35" s="26"/>
+    </row>
+    <row r="36" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="26"/>
+      <c r="K36" s="26"/>
+      <c r="L36" s="26"/>
+      <c r="M36" s="26"/>
+      <c r="N36" s="26"/>
+      <c r="O36" s="26"/>
+      <c r="P36" s="26"/>
+      <c r="Q36" s="26"/>
+    </row>
+    <row r="37" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="26"/>
+      <c r="L37" s="26"/>
+      <c r="M37" s="26"/>
+      <c r="N37" s="26"/>
+      <c r="O37" s="26"/>
+      <c r="P37" s="26"/>
+      <c r="Q37" s="26"/>
+    </row>
+    <row r="38" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="26"/>
+      <c r="K38" s="26"/>
+      <c r="L38" s="26"/>
+      <c r="M38" s="26"/>
+      <c r="N38" s="26"/>
+      <c r="O38" s="26"/>
+      <c r="P38" s="26"/>
+      <c r="Q38" s="26"/>
+    </row>
+    <row r="39" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="26"/>
+      <c r="K39" s="26"/>
+      <c r="L39" s="26"/>
+      <c r="M39" s="26"/>
+      <c r="N39" s="26"/>
+      <c r="O39" s="26"/>
+      <c r="P39" s="26"/>
+      <c r="Q39" s="26"/>
+    </row>
+    <row r="40" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="26"/>
+      <c r="L40" s="26"/>
+      <c r="M40" s="26"/>
+      <c r="N40" s="26"/>
+      <c r="O40" s="26"/>
+      <c r="P40" s="26"/>
+      <c r="Q40" s="26"/>
+    </row>
+    <row r="41" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="26"/>
+      <c r="L41" s="26"/>
+      <c r="M41" s="26"/>
+      <c r="N41" s="26"/>
+      <c r="O41" s="26"/>
+      <c r="P41" s="26"/>
+      <c r="Q41" s="26"/>
+    </row>
+    <row r="42" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="26"/>
+      <c r="K42" s="26"/>
+      <c r="L42" s="26"/>
+      <c r="M42" s="26"/>
+      <c r="N42" s="26"/>
+      <c r="O42" s="26"/>
+      <c r="P42" s="26"/>
+      <c r="Q42" s="26"/>
+    </row>
+    <row r="43" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
+      <c r="K43" s="26"/>
+      <c r="L43" s="26"/>
+      <c r="M43" s="26"/>
+      <c r="N43" s="26"/>
+      <c r="O43" s="26"/>
+      <c r="P43" s="26"/>
+      <c r="Q43" s="26"/>
+    </row>
+    <row r="44" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
+      <c r="K44" s="26"/>
+      <c r="L44" s="26"/>
+      <c r="M44" s="26"/>
+      <c r="N44" s="26"/>
+      <c r="O44" s="26"/>
+      <c r="P44" s="26"/>
+      <c r="Q44" s="26"/>
+    </row>
+    <row r="45" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="26"/>
+      <c r="K45" s="26"/>
+      <c r="L45" s="26"/>
+      <c r="M45" s="26"/>
+      <c r="N45" s="26"/>
+      <c r="O45" s="26"/>
+      <c r="P45" s="26"/>
+      <c r="Q45" s="26"/>
+    </row>
+    <row r="46" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
+      <c r="K46" s="26"/>
+      <c r="L46" s="26"/>
+      <c r="M46" s="26"/>
+      <c r="N46" s="26"/>
+      <c r="O46" s="26"/>
+      <c r="P46" s="26"/>
+      <c r="Q46" s="26"/>
+    </row>
+    <row r="47" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
+      <c r="K47" s="26"/>
+      <c r="L47" s="26"/>
+      <c r="M47" s="26"/>
+      <c r="N47" s="26"/>
+      <c r="O47" s="26"/>
+      <c r="P47" s="26"/>
+      <c r="Q47" s="26"/>
+    </row>
+    <row r="48" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26"/>
+      <c r="G48" s="26"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="26"/>
+      <c r="J48" s="26"/>
+      <c r="K48" s="26"/>
+      <c r="L48" s="26"/>
+      <c r="M48" s="26"/>
+      <c r="N48" s="26"/>
+      <c r="O48" s="26"/>
+      <c r="P48" s="26"/>
+      <c r="Q48" s="26"/>
+    </row>
+    <row r="49" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="26"/>
+      <c r="J49" s="26"/>
+      <c r="K49" s="26"/>
+      <c r="L49" s="26"/>
+      <c r="M49" s="26"/>
+      <c r="N49" s="26"/>
+      <c r="O49" s="26"/>
+      <c r="P49" s="26"/>
+      <c r="Q49" s="26"/>
+    </row>
+    <row r="50" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C50" s="26"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="26"/>
+      <c r="H50" s="26"/>
+      <c r="I50" s="26"/>
+      <c r="J50" s="26"/>
+      <c r="K50" s="26"/>
+      <c r="L50" s="26"/>
+      <c r="M50" s="26"/>
+      <c r="N50" s="26"/>
+      <c r="O50" s="26"/>
+      <c r="P50" s="26"/>
+      <c r="Q50" s="26"/>
+    </row>
+    <row r="51" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="26"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="26"/>
+      <c r="J51" s="26"/>
+      <c r="K51" s="26"/>
+      <c r="L51" s="26"/>
+      <c r="M51" s="26"/>
+      <c r="N51" s="26"/>
+      <c r="O51" s="26"/>
+      <c r="P51" s="26"/>
+      <c r="Q51" s="26"/>
+    </row>
+    <row r="52" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="26"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="26"/>
+      <c r="J52" s="26"/>
+      <c r="K52" s="26"/>
+      <c r="L52" s="26"/>
+      <c r="M52" s="26"/>
+      <c r="N52" s="26"/>
+      <c r="O52" s="26"/>
+      <c r="P52" s="26"/>
+      <c r="Q52" s="26"/>
+    </row>
+    <row r="53" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C53" s="26"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="26"/>
+      <c r="G53" s="26"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="26"/>
+      <c r="J53" s="26"/>
+      <c r="K53" s="26"/>
+      <c r="L53" s="26"/>
+      <c r="M53" s="26"/>
+      <c r="N53" s="26"/>
+      <c r="O53" s="26"/>
+      <c r="P53" s="26"/>
+      <c r="Q53" s="26"/>
+    </row>
+    <row r="54" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="26"/>
+      <c r="H54" s="26"/>
+      <c r="I54" s="26"/>
+      <c r="J54" s="26"/>
+      <c r="K54" s="26"/>
+      <c r="L54" s="26"/>
+      <c r="M54" s="26"/>
+      <c r="N54" s="26"/>
+      <c r="O54" s="26"/>
+      <c r="P54" s="26"/>
+      <c r="Q54" s="26"/>
+    </row>
+    <row r="55" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="26"/>
+      <c r="G55" s="26"/>
+      <c r="H55" s="26"/>
+      <c r="I55" s="26"/>
+      <c r="J55" s="26"/>
+      <c r="K55" s="26"/>
+      <c r="L55" s="26"/>
+      <c r="M55" s="26"/>
+      <c r="N55" s="26"/>
+      <c r="O55" s="26"/>
+      <c r="P55" s="26"/>
+      <c r="Q55" s="26"/>
+    </row>
+    <row r="56" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C56" s="26"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
+      <c r="F56" s="26"/>
+      <c r="G56" s="26"/>
+      <c r="H56" s="26"/>
+      <c r="I56" s="26"/>
+      <c r="J56" s="26"/>
+      <c r="K56" s="26"/>
+      <c r="L56" s="26"/>
+      <c r="M56" s="26"/>
+      <c r="N56" s="26"/>
+      <c r="O56" s="26"/>
+      <c r="P56" s="26"/>
+      <c r="Q56" s="26"/>
+    </row>
+    <row r="57" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C57" s="26"/>
+      <c r="D57" s="26"/>
+      <c r="E57" s="26"/>
+      <c r="F57" s="26"/>
+      <c r="G57" s="26"/>
+      <c r="H57" s="26"/>
+      <c r="I57" s="26"/>
+      <c r="J57" s="26"/>
+      <c r="K57" s="26"/>
+      <c r="L57" s="26"/>
+      <c r="M57" s="26"/>
+      <c r="N57" s="26"/>
+      <c r="O57" s="26"/>
+      <c r="P57" s="26"/>
+      <c r="Q57" s="26"/>
+    </row>
+    <row r="58" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C58" s="26"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="26"/>
+      <c r="F58" s="26"/>
+      <c r="G58" s="26"/>
+      <c r="H58" s="26"/>
+      <c r="I58" s="26"/>
+      <c r="J58" s="26"/>
+      <c r="K58" s="26"/>
+      <c r="L58" s="26"/>
+      <c r="M58" s="26"/>
+      <c r="N58" s="26"/>
+      <c r="O58" s="26"/>
+      <c r="P58" s="26"/>
+      <c r="Q58" s="26"/>
+    </row>
+    <row r="59" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C59" s="26"/>
+      <c r="D59" s="26"/>
+      <c r="E59" s="26"/>
+      <c r="F59" s="26"/>
+      <c r="G59" s="26"/>
+      <c r="H59" s="26"/>
+      <c r="I59" s="26"/>
+      <c r="J59" s="26"/>
+      <c r="K59" s="26"/>
+      <c r="L59" s="26"/>
+      <c r="M59" s="26"/>
+      <c r="N59" s="26"/>
+      <c r="O59" s="26"/>
+      <c r="P59" s="26"/>
+      <c r="Q59" s="26"/>
+    </row>
+    <row r="60" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C60" s="26"/>
+      <c r="D60" s="26"/>
+      <c r="E60" s="26"/>
+      <c r="F60" s="26"/>
+      <c r="G60" s="26"/>
+      <c r="H60" s="26"/>
+      <c r="I60" s="26"/>
+      <c r="J60" s="26"/>
+      <c r="K60" s="26"/>
+      <c r="L60" s="26"/>
+      <c r="M60" s="26"/>
+      <c r="N60" s="26"/>
+      <c r="O60" s="26"/>
+      <c r="P60" s="26"/>
+      <c r="Q60" s="26"/>
+    </row>
+    <row r="61" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C61" s="26"/>
+      <c r="D61" s="26"/>
+      <c r="E61" s="26"/>
+      <c r="F61" s="26"/>
+      <c r="G61" s="26"/>
+      <c r="H61" s="26"/>
+      <c r="I61" s="26"/>
+      <c r="J61" s="26"/>
+      <c r="K61" s="26"/>
+      <c r="L61" s="26"/>
+      <c r="M61" s="26"/>
+      <c r="N61" s="26"/>
+      <c r="O61" s="26"/>
+      <c r="P61" s="26"/>
+      <c r="Q61" s="26"/>
+    </row>
+    <row r="62" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C62" s="26"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="26"/>
+      <c r="G62" s="26"/>
+      <c r="H62" s="26"/>
+      <c r="I62" s="26"/>
+      <c r="J62" s="26"/>
+      <c r="K62" s="26"/>
+      <c r="L62" s="26"/>
+      <c r="M62" s="26"/>
+      <c r="N62" s="26"/>
+      <c r="O62" s="26"/>
+      <c r="P62" s="26"/>
+      <c r="Q62" s="26"/>
+    </row>
+    <row r="63" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C63" s="26"/>
+      <c r="D63" s="26"/>
+      <c r="E63" s="26"/>
+      <c r="F63" s="26"/>
+      <c r="G63" s="26"/>
+      <c r="H63" s="26"/>
+      <c r="I63" s="26"/>
+      <c r="J63" s="26"/>
+      <c r="K63" s="26"/>
+      <c r="L63" s="26"/>
+      <c r="M63" s="26"/>
+      <c r="N63" s="26"/>
+      <c r="O63" s="26"/>
+      <c r="P63" s="26"/>
+      <c r="Q63" s="26"/>
+    </row>
+    <row r="64" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C64" s="26"/>
+      <c r="D64" s="26"/>
+      <c r="E64" s="26"/>
+      <c r="F64" s="26"/>
+      <c r="G64" s="26"/>
+      <c r="H64" s="26"/>
+      <c r="I64" s="26"/>
+      <c r="J64" s="26"/>
+      <c r="K64" s="26"/>
+      <c r="L64" s="26"/>
+      <c r="M64" s="26"/>
+      <c r="N64" s="26"/>
+      <c r="O64" s="26"/>
+      <c r="P64" s="26"/>
+      <c r="Q64" s="26"/>
+    </row>
+    <row r="65" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C65" s="26"/>
+      <c r="D65" s="26"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="26"/>
+      <c r="G65" s="26"/>
+      <c r="H65" s="26"/>
+      <c r="I65" s="26"/>
+      <c r="J65" s="26"/>
+      <c r="K65" s="26"/>
+      <c r="L65" s="26"/>
+      <c r="M65" s="26"/>
+      <c r="N65" s="26"/>
+      <c r="O65" s="26"/>
+      <c r="P65" s="26"/>
+      <c r="Q65" s="26"/>
+    </row>
+    <row r="66" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C66" s="26"/>
+      <c r="D66" s="26"/>
+      <c r="E66" s="26"/>
+      <c r="F66" s="26"/>
+      <c r="G66" s="26"/>
+      <c r="H66" s="26"/>
+      <c r="I66" s="26"/>
+      <c r="J66" s="26"/>
+      <c r="K66" s="26"/>
+      <c r="L66" s="26"/>
+      <c r="M66" s="26"/>
+      <c r="N66" s="26"/>
+      <c r="O66" s="26"/>
+      <c r="P66" s="26"/>
+      <c r="Q66" s="26"/>
+    </row>
+    <row r="67" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C67" s="26"/>
+      <c r="D67" s="26"/>
+      <c r="E67" s="26"/>
+      <c r="F67" s="26"/>
+      <c r="G67" s="26"/>
+      <c r="H67" s="26"/>
+      <c r="I67" s="26"/>
+      <c r="J67" s="26"/>
+      <c r="K67" s="26"/>
+      <c r="L67" s="26"/>
+      <c r="M67" s="26"/>
+      <c r="N67" s="26"/>
+      <c r="O67" s="26"/>
+      <c r="P67" s="26"/>
+      <c r="Q67" s="26"/>
+    </row>
+    <row r="68" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C68" s="26"/>
+      <c r="D68" s="26"/>
+      <c r="E68" s="26"/>
+      <c r="F68" s="26"/>
+      <c r="G68" s="26"/>
+      <c r="H68" s="26"/>
+      <c r="I68" s="26"/>
+      <c r="J68" s="26"/>
+      <c r="K68" s="26"/>
+      <c r="L68" s="26"/>
+      <c r="M68" s="26"/>
+      <c r="N68" s="26"/>
+      <c r="O68" s="26"/>
+      <c r="P68" s="26"/>
+      <c r="Q68" s="26"/>
+    </row>
+    <row r="69" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C69" s="26"/>
+      <c r="D69" s="26"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="26"/>
+      <c r="G69" s="26"/>
+      <c r="H69" s="26"/>
+      <c r="I69" s="26"/>
+      <c r="J69" s="26"/>
+      <c r="K69" s="26"/>
+      <c r="L69" s="26"/>
+      <c r="M69" s="26"/>
+      <c r="N69" s="26"/>
+      <c r="O69" s="26"/>
+      <c r="P69" s="26"/>
+      <c r="Q69" s="26"/>
+    </row>
+    <row r="70" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C70" s="26"/>
+      <c r="D70" s="26"/>
+      <c r="E70" s="26"/>
+      <c r="F70" s="26"/>
+      <c r="G70" s="26"/>
+      <c r="H70" s="26"/>
+      <c r="I70" s="26"/>
+      <c r="J70" s="26"/>
+      <c r="K70" s="26"/>
+      <c r="L70" s="26"/>
+      <c r="M70" s="26"/>
+      <c r="N70" s="26"/>
+      <c r="O70" s="26"/>
+      <c r="P70" s="26"/>
+      <c r="Q70" s="26"/>
+    </row>
+    <row r="71" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C71" s="26"/>
+      <c r="D71" s="26"/>
+      <c r="E71" s="26"/>
+      <c r="F71" s="26"/>
+      <c r="G71" s="26"/>
+      <c r="H71" s="26"/>
+      <c r="I71" s="26"/>
+      <c r="J71" s="26"/>
+      <c r="K71" s="26"/>
+      <c r="L71" s="26"/>
+      <c r="M71" s="26"/>
+      <c r="N71" s="26"/>
+      <c r="O71" s="26"/>
+      <c r="P71" s="26"/>
+      <c r="Q71" s="26"/>
+    </row>
+    <row r="72" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C72" s="26"/>
+      <c r="D72" s="26"/>
+      <c r="E72" s="26"/>
+      <c r="F72" s="26"/>
+      <c r="G72" s="26"/>
+      <c r="H72" s="26"/>
+      <c r="I72" s="26"/>
+      <c r="J72" s="26"/>
+      <c r="K72" s="26"/>
+      <c r="L72" s="26"/>
+      <c r="M72" s="26"/>
+      <c r="N72" s="26"/>
+      <c r="O72" s="26"/>
+      <c r="P72" s="26"/>
+      <c r="Q72" s="26"/>
+    </row>
+    <row r="73" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C73" s="26"/>
+      <c r="D73" s="26"/>
+      <c r="E73" s="26"/>
+      <c r="F73" s="26"/>
+      <c r="G73" s="26"/>
+      <c r="H73" s="26"/>
+      <c r="I73" s="26"/>
+      <c r="J73" s="26"/>
+      <c r="K73" s="26"/>
+      <c r="L73" s="26"/>
+      <c r="M73" s="26"/>
+      <c r="N73" s="26"/>
+      <c r="O73" s="26"/>
+      <c r="P73" s="26"/>
+      <c r="Q73" s="26"/>
+    </row>
+    <row r="74" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C74" s="26"/>
+      <c r="D74" s="26"/>
+      <c r="E74" s="26"/>
+      <c r="F74" s="26"/>
+      <c r="G74" s="26"/>
+      <c r="H74" s="26"/>
+      <c r="I74" s="26"/>
+      <c r="J74" s="26"/>
+      <c r="K74" s="26"/>
+      <c r="L74" s="26"/>
+      <c r="M74" s="26"/>
+      <c r="N74" s="26"/>
+      <c r="O74" s="26"/>
+      <c r="P74" s="26"/>
+      <c r="Q74" s="26"/>
+    </row>
+    <row r="75" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C75" s="26"/>
+      <c r="D75" s="26"/>
+      <c r="E75" s="26"/>
+      <c r="F75" s="26"/>
+      <c r="G75" s="26"/>
+      <c r="H75" s="26"/>
+      <c r="I75" s="26"/>
+      <c r="J75" s="26"/>
+      <c r="K75" s="26"/>
+      <c r="L75" s="26"/>
+      <c r="M75" s="26"/>
+      <c r="N75" s="26"/>
+      <c r="O75" s="26"/>
+      <c r="P75" s="26"/>
+      <c r="Q75" s="26"/>
+    </row>
+    <row r="76" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C76" s="26"/>
+      <c r="D76" s="26"/>
+      <c r="E76" s="26"/>
+      <c r="F76" s="26"/>
+      <c r="G76" s="26"/>
+      <c r="H76" s="26"/>
+      <c r="I76" s="26"/>
+      <c r="J76" s="26"/>
+      <c r="K76" s="26"/>
+      <c r="L76" s="26"/>
+      <c r="M76" s="26"/>
+      <c r="N76" s="26"/>
+      <c r="O76" s="26"/>
+      <c r="P76" s="26"/>
+      <c r="Q76" s="26"/>
+    </row>
+    <row r="77" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C77" s="26"/>
+      <c r="D77" s="26"/>
+      <c r="E77" s="26"/>
+      <c r="F77" s="26"/>
+      <c r="G77" s="26"/>
+      <c r="H77" s="26"/>
+      <c r="I77" s="26"/>
+      <c r="J77" s="26"/>
+      <c r="K77" s="26"/>
+      <c r="L77" s="26"/>
+      <c r="M77" s="26"/>
+      <c r="N77" s="26"/>
+      <c r="O77" s="26"/>
+      <c r="P77" s="26"/>
+      <c r="Q77" s="26"/>
+    </row>
+    <row r="78" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C78" s="26"/>
+      <c r="D78" s="26"/>
+      <c r="E78" s="26"/>
+      <c r="F78" s="26"/>
+      <c r="G78" s="26"/>
+      <c r="H78" s="26"/>
+      <c r="I78" s="26"/>
+      <c r="J78" s="26"/>
+      <c r="K78" s="26"/>
+      <c r="L78" s="26"/>
+      <c r="M78" s="26"/>
+      <c r="N78" s="26"/>
+      <c r="O78" s="26"/>
+      <c r="P78" s="26"/>
+      <c r="Q78" s="26"/>
+    </row>
+    <row r="79" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C79" s="26"/>
+      <c r="D79" s="26"/>
+      <c r="E79" s="26"/>
+      <c r="F79" s="26"/>
+      <c r="G79" s="26"/>
+      <c r="H79" s="26"/>
+      <c r="I79" s="26"/>
+      <c r="J79" s="26"/>
+      <c r="K79" s="26"/>
+      <c r="L79" s="26"/>
+      <c r="M79" s="26"/>
+      <c r="N79" s="26"/>
+      <c r="O79" s="26"/>
+      <c r="P79" s="26"/>
+      <c r="Q79" s="26"/>
+    </row>
+    <row r="80" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C80" s="26"/>
+      <c r="D80" s="26"/>
+      <c r="E80" s="26"/>
+      <c r="F80" s="26"/>
+      <c r="G80" s="26"/>
+      <c r="H80" s="26"/>
+      <c r="I80" s="26"/>
+      <c r="J80" s="26"/>
+      <c r="K80" s="26"/>
+      <c r="L80" s="26"/>
+      <c r="M80" s="26"/>
+      <c r="N80" s="26"/>
+      <c r="O80" s="26"/>
+      <c r="P80" s="26"/>
+      <c r="Q80" s="26"/>
+    </row>
+    <row r="81" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C81" s="26"/>
+      <c r="D81" s="26"/>
+      <c r="E81" s="26"/>
+      <c r="F81" s="26"/>
+      <c r="G81" s="26"/>
+      <c r="H81" s="26"/>
+      <c r="I81" s="26"/>
+      <c r="J81" s="26"/>
+      <c r="K81" s="26"/>
+      <c r="L81" s="26"/>
+      <c r="M81" s="26"/>
+      <c r="N81" s="26"/>
+      <c r="O81" s="26"/>
+      <c r="P81" s="26"/>
+      <c r="Q81" s="26"/>
+    </row>
+    <row r="82" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C82" s="26"/>
+      <c r="D82" s="26"/>
+      <c r="E82" s="26"/>
+      <c r="F82" s="26"/>
+      <c r="G82" s="26"/>
+      <c r="H82" s="26"/>
+      <c r="I82" s="26"/>
+      <c r="J82" s="26"/>
+      <c r="K82" s="26"/>
+      <c r="L82" s="26"/>
+      <c r="M82" s="26"/>
+      <c r="N82" s="26"/>
+      <c r="O82" s="26"/>
+      <c r="P82" s="26"/>
+      <c r="Q82" s="26"/>
+    </row>
+    <row r="83" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C83" s="26"/>
+      <c r="D83" s="26"/>
+      <c r="E83" s="26"/>
+      <c r="F83" s="26"/>
+      <c r="G83" s="26"/>
+      <c r="H83" s="26"/>
+      <c r="I83" s="26"/>
+      <c r="J83" s="26"/>
+      <c r="K83" s="26"/>
+      <c r="L83" s="26"/>
+      <c r="M83" s="26"/>
+      <c r="N83" s="26"/>
+      <c r="O83" s="26"/>
+      <c r="P83" s="26"/>
+      <c r="Q83" s="26"/>
+    </row>
+    <row r="84" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C84" s="26"/>
+      <c r="D84" s="26"/>
+      <c r="E84" s="26"/>
+      <c r="F84" s="26"/>
+      <c r="G84" s="26"/>
+      <c r="H84" s="26"/>
+      <c r="I84" s="26"/>
+      <c r="J84" s="26"/>
+      <c r="K84" s="26"/>
+      <c r="L84" s="26"/>
+      <c r="M84" s="26"/>
+      <c r="N84" s="26"/>
+      <c r="O84" s="26"/>
+      <c r="P84" s="26"/>
+      <c r="Q84" s="26"/>
+    </row>
+    <row r="85" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C85" s="26"/>
+      <c r="D85" s="26"/>
+      <c r="E85" s="26"/>
+      <c r="F85" s="26"/>
+      <c r="G85" s="26"/>
+      <c r="H85" s="26"/>
+      <c r="I85" s="26"/>
+      <c r="J85" s="26"/>
+      <c r="K85" s="26"/>
+      <c r="L85" s="26"/>
+      <c r="M85" s="26"/>
+      <c r="N85" s="26"/>
+      <c r="O85" s="26"/>
+      <c r="P85" s="26"/>
+      <c r="Q85" s="26"/>
+    </row>
+    <row r="86" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C86" s="26"/>
+      <c r="D86" s="26"/>
+      <c r="E86" s="26"/>
+      <c r="F86" s="26"/>
+      <c r="G86" s="26"/>
+      <c r="H86" s="26"/>
+      <c r="I86" s="26"/>
+      <c r="J86" s="26"/>
+      <c r="K86" s="26"/>
+      <c r="L86" s="26"/>
+      <c r="M86" s="26"/>
+      <c r="N86" s="26"/>
+      <c r="O86" s="26"/>
+      <c r="P86" s="26"/>
+      <c r="Q86" s="26"/>
+    </row>
+    <row r="87" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C87" s="26"/>
+      <c r="D87" s="26"/>
+      <c r="E87" s="26"/>
+      <c r="F87" s="26"/>
+      <c r="G87" s="26"/>
+      <c r="H87" s="26"/>
+      <c r="I87" s="26"/>
+      <c r="J87" s="26"/>
+      <c r="K87" s="26"/>
+      <c r="L87" s="26"/>
+      <c r="M87" s="26"/>
+      <c r="N87" s="26"/>
+      <c r="O87" s="26"/>
+      <c r="P87" s="26"/>
+      <c r="Q87" s="26"/>
+    </row>
+    <row r="88" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C88" s="26"/>
+      <c r="D88" s="26"/>
+      <c r="E88" s="26"/>
+      <c r="F88" s="26"/>
+      <c r="G88" s="26"/>
+      <c r="H88" s="26"/>
+      <c r="I88" s="26"/>
+      <c r="J88" s="26"/>
+      <c r="K88" s="26"/>
+      <c r="L88" s="26"/>
+      <c r="M88" s="26"/>
+      <c r="N88" s="26"/>
+      <c r="O88" s="26"/>
+      <c r="P88" s="26"/>
+      <c r="Q88" s="26"/>
+    </row>
+    <row r="89" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C89" s="26"/>
+      <c r="D89" s="26"/>
+      <c r="E89" s="26"/>
+      <c r="F89" s="26"/>
+      <c r="G89" s="26"/>
+      <c r="H89" s="26"/>
+      <c r="I89" s="26"/>
+      <c r="J89" s="26"/>
+      <c r="K89" s="26"/>
+      <c r="L89" s="26"/>
+      <c r="M89" s="26"/>
+      <c r="N89" s="26"/>
+      <c r="O89" s="26"/>
+      <c r="P89" s="26"/>
+      <c r="Q89" s="26"/>
+    </row>
+    <row r="90" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C90" s="26"/>
+      <c r="D90" s="26"/>
+      <c r="E90" s="26"/>
+      <c r="F90" s="26"/>
+      <c r="G90" s="26"/>
+      <c r="H90" s="26"/>
+      <c r="I90" s="26"/>
+      <c r="J90" s="26"/>
+      <c r="K90" s="26"/>
+      <c r="L90" s="26"/>
+      <c r="M90" s="26"/>
+      <c r="N90" s="26"/>
+      <c r="O90" s="26"/>
+      <c r="P90" s="26"/>
+      <c r="Q90" s="26"/>
+    </row>
+    <row r="91" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C91" s="26"/>
+      <c r="D91" s="26"/>
+      <c r="E91" s="26"/>
+      <c r="F91" s="26"/>
+      <c r="G91" s="26"/>
+      <c r="H91" s="26"/>
+      <c r="I91" s="26"/>
+      <c r="J91" s="26"/>
+      <c r="K91" s="26"/>
+      <c r="L91" s="26"/>
+      <c r="M91" s="26"/>
+      <c r="N91" s="26"/>
+      <c r="O91" s="26"/>
+      <c r="P91" s="26"/>
+      <c r="Q91" s="26"/>
+    </row>
+    <row r="92" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C92" s="26"/>
+      <c r="D92" s="26"/>
+      <c r="E92" s="26"/>
+      <c r="F92" s="26"/>
+      <c r="G92" s="26"/>
+      <c r="H92" s="26"/>
+      <c r="I92" s="26"/>
+      <c r="J92" s="26"/>
+      <c r="K92" s="26"/>
+      <c r="L92" s="26"/>
+      <c r="M92" s="26"/>
+      <c r="N92" s="26"/>
+      <c r="O92" s="26"/>
+      <c r="P92" s="26"/>
+      <c r="Q92" s="26"/>
+    </row>
+    <row r="93" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C93" s="26"/>
+      <c r="D93" s="26"/>
+      <c r="E93" s="26"/>
+      <c r="F93" s="26"/>
+      <c r="G93" s="26"/>
+      <c r="H93" s="26"/>
+      <c r="I93" s="26"/>
+      <c r="J93" s="26"/>
+      <c r="K93" s="26"/>
+      <c r="L93" s="26"/>
+      <c r="M93" s="26"/>
+      <c r="N93" s="26"/>
+      <c r="O93" s="26"/>
+      <c r="P93" s="26"/>
+      <c r="Q93" s="26"/>
+    </row>
+    <row r="94" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C94" s="26"/>
+      <c r="D94" s="26"/>
+      <c r="E94" s="26"/>
+      <c r="F94" s="26"/>
+      <c r="G94" s="26"/>
+      <c r="H94" s="26"/>
+      <c r="I94" s="26"/>
+      <c r="J94" s="26"/>
+      <c r="K94" s="26"/>
+      <c r="L94" s="26"/>
+      <c r="M94" s="26"/>
+      <c r="N94" s="26"/>
+      <c r="O94" s="26"/>
+      <c r="P94" s="26"/>
+      <c r="Q94" s="26"/>
+    </row>
+    <row r="95" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C95" s="26"/>
+      <c r="D95" s="26"/>
+      <c r="E95" s="26"/>
+      <c r="F95" s="26"/>
+      <c r="G95" s="26"/>
+      <c r="H95" s="26"/>
+      <c r="I95" s="26"/>
+      <c r="J95" s="26"/>
+      <c r="K95" s="26"/>
+      <c r="L95" s="26"/>
+      <c r="M95" s="26"/>
+      <c r="N95" s="26"/>
+      <c r="O95" s="26"/>
+      <c r="P95" s="26"/>
+      <c r="Q95" s="26"/>
+    </row>
+    <row r="96" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C96" s="26"/>
+      <c r="D96" s="26"/>
+      <c r="E96" s="26"/>
+      <c r="F96" s="26"/>
+      <c r="G96" s="26"/>
+      <c r="H96" s="26"/>
+      <c r="I96" s="26"/>
+      <c r="J96" s="26"/>
+      <c r="K96" s="26"/>
+      <c r="L96" s="26"/>
+      <c r="M96" s="26"/>
+      <c r="N96" s="26"/>
+      <c r="O96" s="26"/>
+      <c r="P96" s="26"/>
+      <c r="Q96" s="26"/>
+    </row>
+    <row r="97" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C97" s="26"/>
+      <c r="D97" s="26"/>
+      <c r="E97" s="26"/>
+      <c r="F97" s="26"/>
+      <c r="G97" s="26"/>
+      <c r="H97" s="26"/>
+      <c r="I97" s="26"/>
+      <c r="J97" s="26"/>
+      <c r="K97" s="26"/>
+      <c r="L97" s="26"/>
+      <c r="M97" s="26"/>
+      <c r="N97" s="26"/>
+      <c r="O97" s="26"/>
+      <c r="P97" s="26"/>
+      <c r="Q97" s="26"/>
+    </row>
+    <row r="98" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C98" s="26"/>
+      <c r="D98" s="26"/>
+      <c r="E98" s="26"/>
+      <c r="F98" s="26"/>
+      <c r="G98" s="26"/>
+      <c r="H98" s="26"/>
+      <c r="I98" s="26"/>
+      <c r="J98" s="26"/>
+      <c r="K98" s="26"/>
+      <c r="L98" s="26"/>
+      <c r="M98" s="26"/>
+      <c r="N98" s="26"/>
+      <c r="O98" s="26"/>
+      <c r="P98" s="26"/>
+      <c r="Q98" s="26"/>
+    </row>
+    <row r="99" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C99" s="26"/>
+      <c r="D99" s="26"/>
+      <c r="E99" s="26"/>
+      <c r="F99" s="26"/>
+      <c r="G99" s="26"/>
+      <c r="H99" s="26"/>
+      <c r="I99" s="26"/>
+      <c r="J99" s="26"/>
+      <c r="K99" s="26"/>
+      <c r="L99" s="26"/>
+      <c r="M99" s="26"/>
+      <c r="N99" s="26"/>
+      <c r="O99" s="26"/>
+      <c r="P99" s="26"/>
+      <c r="Q99" s="26"/>
+    </row>
+    <row r="100" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C100" s="26"/>
+      <c r="D100" s="26"/>
+      <c r="E100" s="26"/>
+      <c r="F100" s="26"/>
+      <c r="G100" s="26"/>
+      <c r="H100" s="26"/>
+      <c r="I100" s="26"/>
+      <c r="J100" s="26"/>
+      <c r="K100" s="26"/>
+      <c r="L100" s="26"/>
+      <c r="M100" s="26"/>
+      <c r="N100" s="26"/>
+      <c r="O100" s="26"/>
+      <c r="P100" s="26"/>
+      <c r="Q100" s="26"/>
+    </row>
+    <row r="101" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C101" s="26"/>
+      <c r="D101" s="26"/>
+      <c r="E101" s="26"/>
+      <c r="F101" s="26"/>
+      <c r="G101" s="26"/>
+      <c r="H101" s="26"/>
+      <c r="I101" s="26"/>
+      <c r="J101" s="26"/>
+      <c r="K101" s="26"/>
+      <c r="L101" s="26"/>
+      <c r="M101" s="26"/>
+      <c r="N101" s="26"/>
+      <c r="O101" s="26"/>
+      <c r="P101" s="26"/>
+      <c r="Q101" s="26"/>
+    </row>
+    <row r="102" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C102" s="26"/>
+      <c r="D102" s="26"/>
+      <c r="E102" s="26"/>
+      <c r="F102" s="26"/>
+      <c r="G102" s="26"/>
+      <c r="H102" s="26"/>
+      <c r="I102" s="26"/>
+      <c r="J102" s="26"/>
+      <c r="K102" s="26"/>
+      <c r="L102" s="26"/>
+      <c r="M102" s="26"/>
+      <c r="N102" s="26"/>
+      <c r="O102" s="26"/>
+      <c r="P102" s="26"/>
+      <c r="Q102" s="26"/>
+    </row>
+    <row r="103" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C103" s="26"/>
+      <c r="D103" s="26"/>
+      <c r="E103" s="26"/>
+      <c r="F103" s="26"/>
+      <c r="G103" s="26"/>
+      <c r="H103" s="26"/>
+      <c r="I103" s="26"/>
+      <c r="J103" s="26"/>
+      <c r="K103" s="26"/>
+      <c r="L103" s="26"/>
+      <c r="M103" s="26"/>
+      <c r="N103" s="26"/>
+      <c r="O103" s="26"/>
+      <c r="P103" s="26"/>
+      <c r="Q103" s="26"/>
+    </row>
+    <row r="104" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C104" s="26"/>
+      <c r="D104" s="26"/>
+      <c r="E104" s="26"/>
+      <c r="F104" s="26"/>
+      <c r="G104" s="26"/>
+      <c r="H104" s="26"/>
+      <c r="I104" s="26"/>
+      <c r="J104" s="26"/>
+      <c r="K104" s="26"/>
+      <c r="L104" s="26"/>
+      <c r="M104" s="26"/>
+      <c r="N104" s="26"/>
+      <c r="O104" s="26"/>
+      <c r="P104" s="26"/>
+      <c r="Q104" s="26"/>
+    </row>
+    <row r="105" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C105" s="26"/>
+      <c r="D105" s="26"/>
+      <c r="E105" s="26"/>
+      <c r="F105" s="26"/>
+      <c r="G105" s="26"/>
+      <c r="H105" s="26"/>
+      <c r="I105" s="26"/>
+      <c r="J105" s="26"/>
+      <c r="K105" s="26"/>
+      <c r="L105" s="26"/>
+      <c r="M105" s="26"/>
+      <c r="N105" s="26"/>
+      <c r="O105" s="26"/>
+      <c r="P105" s="26"/>
+      <c r="Q105" s="26"/>
+    </row>
+    <row r="106" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C106" s="26"/>
+      <c r="D106" s="26"/>
+      <c r="E106" s="26"/>
+      <c r="F106" s="26"/>
+      <c r="G106" s="26"/>
+      <c r="H106" s="26"/>
+      <c r="I106" s="26"/>
+      <c r="J106" s="26"/>
+      <c r="K106" s="26"/>
+      <c r="L106" s="26"/>
+      <c r="M106" s="26"/>
+      <c r="N106" s="26"/>
+      <c r="O106" s="26"/>
+      <c r="P106" s="26"/>
+      <c r="Q106" s="26"/>
+    </row>
+    <row r="107" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C107" s="26"/>
+      <c r="D107" s="26"/>
+      <c r="E107" s="26"/>
+      <c r="F107" s="26"/>
+      <c r="G107" s="26"/>
+      <c r="H107" s="26"/>
+      <c r="I107" s="26"/>
+      <c r="J107" s="26"/>
+      <c r="K107" s="26"/>
+      <c r="L107" s="26"/>
+      <c r="M107" s="26"/>
+      <c r="N107" s="26"/>
+      <c r="O107" s="26"/>
+      <c r="P107" s="26"/>
+      <c r="Q107" s="26"/>
+    </row>
+    <row r="108" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C108" s="26"/>
+      <c r="D108" s="26"/>
+      <c r="E108" s="26"/>
+      <c r="F108" s="26"/>
+      <c r="G108" s="26"/>
+      <c r="H108" s="26"/>
+      <c r="I108" s="26"/>
+      <c r="J108" s="26"/>
+      <c r="K108" s="26"/>
+      <c r="L108" s="26"/>
+      <c r="M108" s="26"/>
+      <c r="N108" s="26"/>
+      <c r="O108" s="26"/>
+      <c r="P108" s="26"/>
+      <c r="Q108" s="26"/>
+    </row>
+    <row r="109" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C109" s="26"/>
+      <c r="D109" s="26"/>
+      <c r="E109" s="26"/>
+      <c r="F109" s="26"/>
+      <c r="G109" s="26"/>
+      <c r="H109" s="26"/>
+      <c r="I109" s="26"/>
+      <c r="J109" s="26"/>
+      <c r="K109" s="26"/>
+      <c r="L109" s="26"/>
+      <c r="M109" s="26"/>
+      <c r="N109" s="26"/>
+      <c r="O109" s="26"/>
+      <c r="P109" s="26"/>
+      <c r="Q109" s="26"/>
+    </row>
+    <row r="110" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C110" s="26"/>
+      <c r="D110" s="26"/>
+      <c r="E110" s="26"/>
+      <c r="F110" s="26"/>
+      <c r="G110" s="26"/>
+      <c r="H110" s="26"/>
+      <c r="I110" s="26"/>
+      <c r="J110" s="26"/>
+      <c r="K110" s="26"/>
+      <c r="L110" s="26"/>
+      <c r="M110" s="26"/>
+      <c r="N110" s="26"/>
+      <c r="O110" s="26"/>
+      <c r="P110" s="26"/>
+      <c r="Q110" s="26"/>
+    </row>
+    <row r="111" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C111" s="26"/>
+      <c r="D111" s="26"/>
+      <c r="E111" s="26"/>
+      <c r="F111" s="26"/>
+      <c r="G111" s="26"/>
+      <c r="H111" s="26"/>
+      <c r="I111" s="26"/>
+      <c r="J111" s="26"/>
+      <c r="K111" s="26"/>
+      <c r="L111" s="26"/>
+      <c r="M111" s="26"/>
+      <c r="N111" s="26"/>
+      <c r="O111" s="26"/>
+      <c r="P111" s="26"/>
+      <c r="Q111" s="26"/>
+    </row>
+    <row r="112" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C112" s="26"/>
+      <c r="D112" s="26"/>
+      <c r="E112" s="26"/>
+      <c r="F112" s="26"/>
+      <c r="G112" s="26"/>
+      <c r="H112" s="26"/>
+      <c r="I112" s="26"/>
+      <c r="J112" s="26"/>
+      <c r="K112" s="26"/>
+      <c r="L112" s="26"/>
+      <c r="M112" s="26"/>
+      <c r="N112" s="26"/>
+      <c r="O112" s="26"/>
+      <c r="P112" s="26"/>
+      <c r="Q112" s="26"/>
+    </row>
+    <row r="113" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C113" s="26"/>
+      <c r="D113" s="26"/>
+      <c r="E113" s="26"/>
+      <c r="F113" s="26"/>
+      <c r="G113" s="26"/>
+      <c r="H113" s="26"/>
+      <c r="I113" s="26"/>
+      <c r="J113" s="26"/>
+      <c r="K113" s="26"/>
+      <c r="L113" s="26"/>
+      <c r="M113" s="26"/>
+      <c r="N113" s="26"/>
+      <c r="O113" s="26"/>
+      <c r="P113" s="26"/>
+      <c r="Q113" s="26"/>
+    </row>
+    <row r="114" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C114" s="26"/>
+      <c r="D114" s="26"/>
+      <c r="E114" s="26"/>
+      <c r="F114" s="26"/>
+      <c r="G114" s="26"/>
+      <c r="H114" s="26"/>
+      <c r="I114" s="26"/>
+      <c r="J114" s="26"/>
+      <c r="K114" s="26"/>
+      <c r="L114" s="26"/>
+      <c r="M114" s="26"/>
+      <c r="N114" s="26"/>
+      <c r="O114" s="26"/>
+      <c r="P114" s="26"/>
+      <c r="Q114" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14896,7 +16203,7 @@
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="J19" sqref="J14:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17796,7 +19103,7 @@
   <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>